<commit_message>
Updated XLS source file parse fields
Signed-off-by: tc45 <33063166+tc45@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/GetInventory - Default.xlsx
+++ b/GetInventory - Default.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tony\PycharmProjects\NetDevOps-GetInventory\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E0D20E9-9352-49E4-AE61-B200D219405F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88661E68-A3B8-4C70-A3C8-2595D05C3AD0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="154">
   <si>
     <t>Username</t>
   </si>
@@ -503,6 +503,12 @@
   </si>
   <si>
     <t>VLAN IF - Active</t>
+  </si>
+  <si>
+    <t>cisco_nxos</t>
+  </si>
+  <si>
+    <t>cisco_ios</t>
   </si>
 </sst>
 </file>
@@ -1152,7 +1158,7 @@
         <v>31</v>
       </c>
       <c r="C9" t="s">
-        <v>124</v>
+        <v>152</v>
       </c>
     </row>
     <row r="10" spans="1:49" x14ac:dyDescent="0.25">
@@ -1163,7 +1169,7 @@
         <v>31</v>
       </c>
       <c r="C10" t="s">
-        <v>124</v>
+        <v>153</v>
       </c>
       <c r="E10">
         <v>2222</v>
@@ -1176,9 +1182,6 @@
       <c r="B11" t="s">
         <v>31</v>
       </c>
-      <c r="C11" t="s">
-        <v>124</v>
-      </c>
       <c r="D11" t="s">
         <v>13</v>
       </c>
@@ -1189,9 +1192,6 @@
       </c>
       <c r="B12" t="s">
         <v>31</v>
-      </c>
-      <c r="C12" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="13" spans="1:49" x14ac:dyDescent="0.25">
@@ -1222,8 +1222,8 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B8:B998" xr:uid="{9E79B49A-5F92-4A71-B3FE-85893E55E1CA}">
       <formula1>"Yes,No,Completed"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C8:C1132" xr:uid="{4F3676CE-4307-4242-A50B-53311B37CE11}">
-      <formula1>"cisco-ios, cisco-nxos, autodetect"</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C8:C1199" xr:uid="{ECF68FFA-6D07-4745-B142-7976EE519DCC}">
+      <formula1>"cisco_ios, cisco_nxos, autodetect"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added VRF Parser for route tables and ARP tables.
Signed-off-by: tc45 <33063166+tc45@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/GetInventory - Default.xlsx
+++ b/GetInventory - Default.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tony\PycharmProjects\NetDevOps-GetInventory\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88661E68-A3B8-4C70-A3C8-2595D05C3AD0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AA71943-0BC8-4C90-9C16-6D425A1E56CB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="151">
   <si>
     <t>Username</t>
   </si>
@@ -63,9 +63,6 @@
     <t>Output Directory</t>
   </si>
   <si>
-    <t>C:\temp\Test_ParseIT\</t>
-  </si>
-  <si>
     <t>Output Name</t>
   </si>
   <si>
@@ -87,9 +84,6 @@
     <t>Connection Error</t>
   </si>
   <si>
-    <t>telnet</t>
-  </si>
-  <si>
     <t>show clock</t>
   </si>
   <si>
@@ -172,21 +166,6 @@
   </si>
   <si>
     <t>Uptime</t>
-  </si>
-  <si>
-    <t>172.16.255.101</t>
-  </si>
-  <si>
-    <t>172.16.255.102</t>
-  </si>
-  <si>
-    <t>172.16.255.4</t>
-  </si>
-  <si>
-    <t>172.16.255.8</t>
-  </si>
-  <si>
-    <t>172.16.255.5</t>
   </si>
   <si>
     <t>Local Port</t>
@@ -421,21 +400,9 @@
 (defaults to cisco_ios)</t>
   </si>
   <si>
-    <t>autodetect</t>
-  </si>
-  <si>
     <t>IP/DNS Host</t>
   </si>
   <si>
-    <t>LABTEST</t>
-  </si>
-  <si>
-    <t>192.168.1.1</t>
-  </si>
-  <si>
-    <t>test1</t>
-  </si>
-  <si>
     <t>show ip bgp</t>
   </si>
   <si>
@@ -505,10 +472,34 @@
     <t>VLAN IF - Active</t>
   </si>
   <si>
+    <t>C:\temp\SHOW_VRF\</t>
+  </si>
+  <si>
+    <t>showvrf</t>
+  </si>
+  <si>
+    <t>172.31.22.129</t>
+  </si>
+  <si>
+    <t>172.31.22.130</t>
+  </si>
+  <si>
+    <t>172.31.22.131</t>
+  </si>
+  <si>
+    <t>172.31.22.134</t>
+  </si>
+  <si>
     <t>cisco_nxos</t>
   </si>
   <si>
-    <t>cisco_ios</t>
+    <t>172.31.22.128</t>
+  </si>
+  <si>
+    <t>show vrf</t>
+  </si>
+  <si>
+    <t>show ip route vrf x</t>
   </si>
 </sst>
 </file>
@@ -908,10 +899,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AW14"/>
+  <dimension ref="A1:AW12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -975,36 +966,36 @@
         <v>4</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>5</v>
+        <v>141</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
     </row>
     <row r="5" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>126</v>
+        <v>142</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
     </row>
     <row r="7" spans="1:49" ht="113.25" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="D7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>9</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>0</v>
@@ -1013,198 +1004,176 @@
         <v>2</v>
       </c>
       <c r="H7" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="M7" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="N7" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="O7" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="P7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q7" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="R7" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="S7" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="T7" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="U7" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="V7" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="W7" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="I7" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="J7" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="K7" s="2" t="s">
+      <c r="X7" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="Y7" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="L7" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="M7" s="2" t="s">
+      <c r="Z7" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="AA7" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="AB7" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="AC7" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="AD7" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="AE7" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="AF7" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="AG7" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="AH7" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="AI7" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="AJ7" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="AK7" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="AL7" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="AM7" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="AN7" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="AO7" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="AP7" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="AQ7" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="N7" s="2" t="s">
+      <c r="AR7" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="O7" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="P7" s="2" t="s">
+      <c r="AS7" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="AT7" s="2" t="s">
         <v>11</v>
-      </c>
-      <c r="Q7" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="R7" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="S7" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="T7" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="U7" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="V7" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="W7" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="X7" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="Y7" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="Z7" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="AA7" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="AB7" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="AC7" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="AD7" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="AE7" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="AF7" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="AG7" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="AH7" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="AI7" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="AJ7" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="AK7" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="AL7" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="AM7" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="AN7" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="AO7" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="AP7" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="AQ7" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="AR7" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="AS7" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="AT7" s="2" t="s">
-        <v>12</v>
       </c>
       <c r="AU7" s="2" t="s">
         <v>4</v>
       </c>
       <c r="AV7" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="AW7" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>44</v>
+        <v>144</v>
       </c>
       <c r="B8" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C8" t="s">
-        <v>124</v>
+        <v>147</v>
       </c>
     </row>
     <row r="9" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>46</v>
+        <v>145</v>
       </c>
       <c r="B9" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C9" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
     </row>
     <row r="10" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>45</v>
+        <v>146</v>
       </c>
       <c r="B10" t="s">
-        <v>31</v>
-      </c>
-      <c r="C10" t="s">
-        <v>153</v>
-      </c>
-      <c r="E10">
-        <v>2222</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>42</v>
+        <v>143</v>
       </c>
       <c r="B11" t="s">
-        <v>31</v>
-      </c>
-      <c r="D11" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>43</v>
+        <v>148</v>
       </c>
       <c r="B12" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="13" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>127</v>
-      </c>
-      <c r="B13" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="14" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>128</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -1216,13 +1185,13 @@
     <mergeCell ref="B5:D5"/>
   </mergeCells>
   <dataValidations count="3">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B999:B1233 D8:D15" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B998:B1232 D8:D15" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"ssh, telnet"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B8:B998" xr:uid="{9E79B49A-5F92-4A71-B3FE-85893E55E1CA}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B8:B997" xr:uid="{9E79B49A-5F92-4A71-B3FE-85893E55E1CA}">
       <formula1>"Yes,No,Completed"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C8:C1199" xr:uid="{ECF68FFA-6D07-4745-B142-7976EE519DCC}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C8:C1198" xr:uid="{ECF68FFA-6D07-4745-B142-7976EE519DCC}">
       <formula1>"cisco_ios, cisco_nxos, autodetect"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1247,13 +1216,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B1" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="C1" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
     </row>
   </sheetData>
@@ -1283,25 +1252,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B1" t="s">
-        <v>131</v>
+        <v>120</v>
       </c>
       <c r="C1" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="D1" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="E1" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="F1" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="G1" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -1327,19 +1296,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B1" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="C1" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="D1" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="E1" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
     </row>
   </sheetData>
@@ -1366,28 +1335,28 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B1" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="C1" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="D1" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="E1" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="F1" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="G1" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="H1" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
     </row>
   </sheetData>
@@ -1435,97 +1404,97 @@
   <sheetData>
     <row r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E1" t="s">
+        <v>104</v>
+      </c>
+      <c r="F1" t="s">
+        <v>120</v>
+      </c>
+      <c r="G1" t="s">
+        <v>48</v>
+      </c>
+      <c r="H1" t="s">
         <v>7</v>
       </c>
-      <c r="B1" t="s">
+      <c r="I1" t="s">
+        <v>70</v>
+      </c>
+      <c r="J1" t="s">
+        <v>47</v>
+      </c>
+      <c r="K1" t="s">
+        <v>67</v>
+      </c>
+      <c r="L1" t="s">
+        <v>68</v>
+      </c>
+      <c r="M1" t="s">
+        <v>69</v>
+      </c>
+      <c r="N1" t="s">
+        <v>72</v>
+      </c>
+      <c r="O1" t="s">
+        <v>49</v>
+      </c>
+      <c r="P1" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="R1" t="s">
         <v>53</v>
       </c>
-      <c r="C1" t="s">
-        <v>78</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="S1" t="s">
+        <v>54</v>
+      </c>
+      <c r="T1" t="s">
+        <v>55</v>
+      </c>
+      <c r="U1" t="s">
+        <v>56</v>
+      </c>
+      <c r="V1" t="s">
+        <v>57</v>
+      </c>
+      <c r="W1" t="s">
         <v>58</v>
       </c>
-      <c r="E1" t="s">
-        <v>111</v>
-      </c>
-      <c r="F1" t="s">
-        <v>131</v>
-      </c>
-      <c r="G1" t="s">
-        <v>55</v>
-      </c>
-      <c r="H1" t="s">
-        <v>8</v>
-      </c>
-      <c r="I1" t="s">
-        <v>77</v>
-      </c>
-      <c r="J1" t="s">
-        <v>54</v>
-      </c>
-      <c r="K1" t="s">
-        <v>74</v>
-      </c>
-      <c r="L1" t="s">
-        <v>75</v>
-      </c>
-      <c r="M1" t="s">
-        <v>76</v>
-      </c>
-      <c r="N1" t="s">
-        <v>79</v>
-      </c>
-      <c r="O1" t="s">
-        <v>56</v>
-      </c>
-      <c r="P1" t="s">
-        <v>57</v>
-      </c>
-      <c r="Q1" s="1" t="s">
+      <c r="X1" t="s">
         <v>59</v>
       </c>
-      <c r="R1" t="s">
+      <c r="Y1" t="s">
         <v>60</v>
       </c>
-      <c r="S1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="T1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="U1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="V1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="W1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="X1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>66</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>67</v>
-      </c>
-      <c r="Z1" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="AA1" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="AB1" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="AC1" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="AD1" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="AE1" s="1" t="s">
-        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -1555,31 +1524,31 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B1" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="C1" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="D1" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="E1" t="s">
-        <v>133</v>
+        <v>122</v>
       </c>
       <c r="F1" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="G1" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="H1" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="I1" t="s">
-        <v>134</v>
+        <v>123</v>
       </c>
     </row>
   </sheetData>
@@ -1609,37 +1578,37 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C1" t="s">
         <v>7</v>
       </c>
-      <c r="B1" t="s">
-        <v>131</v>
-      </c>
-      <c r="C1" t="s">
-        <v>8</v>
-      </c>
       <c r="D1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H1" t="s">
+        <v>38</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="J1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="G1" t="s">
+      <c r="K1" t="s">
         <v>39</v>
-      </c>
-      <c r="H1" t="s">
-        <v>40</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="K1" t="s">
-        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -1650,97 +1619,107 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E71063F6-A136-491C-B6BE-7CD0E59E5434}">
-  <dimension ref="A1:A17"/>
+  <dimension ref="A1:A19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>129</v>
+        <v>118</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>130</v>
+        <v>119</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>150</v>
       </c>
     </row>
   </sheetData>
@@ -1767,80 +1746,80 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" t="s">
         <v>29</v>
-      </c>
-      <c r="B7" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B8" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="B9" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated spreadsheet with new columns, BGP, Inventory, LLDP, and Settings.
Signed-off-by: tc45 <33063166+tc45@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/GetInventory - Default.xlsx
+++ b/GetInventory - Default.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tony\PycharmProjects\NetDevOps-GetInventory\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94EF73CF-F4B3-4D76-BF48-8445D4772B8E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9132195-396D-404C-9804-9D285B626D54}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="849" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29190" yWindow="390" windowWidth="21585" windowHeight="12405" tabRatio="849" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="232">
   <si>
     <t>Username</t>
   </si>
@@ -747,6 +747,9 @@
   </si>
   <si>
     <t>172.31.22.134</t>
+  </si>
+  <si>
+    <t>IOS Filename</t>
   </si>
 </sst>
 </file>
@@ -908,10 +911,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1229,10 +1232,10 @@
   <sheetPr>
     <tabColor theme="5" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="A1:BB68"/>
+  <dimension ref="A1:BC68"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1251,84 +1254,85 @@
     <col min="12" max="12" width="15.42578125" customWidth="1"/>
     <col min="14" max="14" width="16" customWidth="1"/>
     <col min="15" max="15" width="20" customWidth="1"/>
-    <col min="16" max="16" width="41.28515625" customWidth="1"/>
-    <col min="17" max="33" width="4.28515625" customWidth="1"/>
-    <col min="34" max="42" width="4.42578125" customWidth="1"/>
-    <col min="43" max="43" width="4.42578125" style="19" customWidth="1"/>
-    <col min="44" max="44" width="4.42578125" customWidth="1"/>
-    <col min="46" max="46" width="16.7109375" customWidth="1"/>
-    <col min="47" max="47" width="74.28515625" customWidth="1"/>
-    <col min="48" max="48" width="54.5703125" customWidth="1"/>
-    <col min="49" max="49" width="37.28515625" customWidth="1"/>
-    <col min="50" max="50" width="37.85546875" customWidth="1"/>
+    <col min="16" max="16" width="16" style="24" customWidth="1"/>
+    <col min="17" max="17" width="51.140625" style="24" customWidth="1"/>
+    <col min="18" max="34" width="4.28515625" customWidth="1"/>
+    <col min="35" max="43" width="4.42578125" customWidth="1"/>
+    <col min="44" max="44" width="4.42578125" style="19" customWidth="1"/>
+    <col min="45" max="45" width="4.42578125" customWidth="1"/>
+    <col min="47" max="47" width="16.7109375" customWidth="1"/>
+    <col min="48" max="48" width="74.28515625" customWidth="1"/>
+    <col min="49" max="49" width="54.5703125" customWidth="1"/>
+    <col min="50" max="50" width="37.28515625" customWidth="1"/>
+    <col min="51" max="51" width="37.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="26" t="s">
         <v>221</v>
       </c>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-    </row>
-    <row r="2" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+    </row>
+    <row r="2" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="26" t="s">
         <v>221</v>
       </c>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-    </row>
-    <row r="3" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="26"/>
+    </row>
+    <row r="3" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="25" t="s">
+      <c r="B3" s="26" t="s">
         <v>221</v>
       </c>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
-    </row>
-    <row r="4" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="26"/>
+      <c r="G3" s="26"/>
+    </row>
+    <row r="4" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="25" t="s">
+      <c r="B4" s="26" t="s">
         <v>222</v>
       </c>
-      <c r="C4" s="25"/>
-      <c r="D4" s="25"/>
-      <c r="E4" s="25"/>
-      <c r="F4" s="25"/>
-      <c r="G4" s="25"/>
-    </row>
-    <row r="5" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="C4" s="26"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="26"/>
+      <c r="F4" s="26"/>
+      <c r="G4" s="26"/>
+    </row>
+    <row r="5" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="25" t="s">
+      <c r="B5" s="26" t="s">
         <v>223</v>
       </c>
-      <c r="C5" s="25"/>
-      <c r="D5" s="25"/>
-      <c r="E5" s="25"/>
-      <c r="F5" s="25"/>
-      <c r="G5" s="25"/>
-    </row>
-    <row r="7" spans="1:54" ht="113.25" x14ac:dyDescent="0.25">
+      <c r="C5" s="26"/>
+      <c r="D5" s="26"/>
+      <c r="E5" s="26"/>
+      <c r="F5" s="26"/>
+      <c r="G5" s="26"/>
+    </row>
+    <row r="7" spans="1:55" ht="113.25" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>200</v>
       </c>
@@ -1377,122 +1381,125 @@
       <c r="P7" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="Q7" s="21" t="s">
+      <c r="Q7" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="R7" s="21" t="s">
         <v>84</v>
       </c>
-      <c r="R7" s="21" t="s">
+      <c r="S7" s="21" t="s">
         <v>127</v>
       </c>
-      <c r="S7" s="21" t="s">
+      <c r="T7" s="21" t="s">
         <v>85</v>
       </c>
-      <c r="T7" s="21" t="s">
+      <c r="U7" s="21" t="s">
         <v>128</v>
       </c>
-      <c r="U7" s="21" t="s">
+      <c r="V7" s="21" t="s">
         <v>86</v>
       </c>
-      <c r="V7" s="21" t="s">
+      <c r="W7" s="21" t="s">
         <v>129</v>
       </c>
-      <c r="W7" s="21" t="s">
+      <c r="X7" s="21" t="s">
         <v>87</v>
       </c>
-      <c r="X7" s="21" t="s">
+      <c r="Y7" s="21" t="s">
         <v>130</v>
       </c>
-      <c r="Y7" s="21" t="s">
+      <c r="Z7" s="21" t="s">
         <v>88</v>
       </c>
-      <c r="Z7" s="21" t="s">
+      <c r="AA7" s="21" t="s">
         <v>131</v>
       </c>
-      <c r="AA7" s="21" t="s">
+      <c r="AB7" s="21" t="s">
         <v>92</v>
       </c>
-      <c r="AB7" s="21" t="s">
+      <c r="AC7" s="21" t="s">
         <v>132</v>
       </c>
-      <c r="AC7" s="21" t="s">
+      <c r="AD7" s="21" t="s">
         <v>93</v>
       </c>
-      <c r="AD7" s="21" t="s">
+      <c r="AE7" s="21" t="s">
         <v>133</v>
       </c>
-      <c r="AE7" s="21" t="s">
+      <c r="AF7" s="21" t="s">
         <v>94</v>
       </c>
-      <c r="AF7" s="21" t="s">
+      <c r="AG7" s="21" t="s">
         <v>134</v>
       </c>
-      <c r="AG7" s="21" t="s">
+      <c r="AH7" s="21" t="s">
         <v>109</v>
       </c>
-      <c r="AH7" s="21" t="s">
+      <c r="AI7" s="21" t="s">
         <v>135</v>
       </c>
-      <c r="AI7" s="21" t="s">
+      <c r="AJ7" s="21" t="s">
         <v>121</v>
       </c>
-      <c r="AJ7" s="21" t="s">
+      <c r="AK7" s="21" t="s">
         <v>124</v>
       </c>
-      <c r="AK7" s="21" t="s">
+      <c r="AL7" s="21" t="s">
         <v>122</v>
       </c>
-      <c r="AL7" s="21" t="s">
+      <c r="AM7" s="21" t="s">
         <v>125</v>
       </c>
-      <c r="AM7" s="21" t="s">
+      <c r="AN7" s="21" t="s">
         <v>123</v>
       </c>
-      <c r="AN7" s="21" t="s">
+      <c r="AO7" s="21" t="s">
         <v>126</v>
       </c>
-      <c r="AO7" s="21" t="s">
+      <c r="AP7" s="21" t="s">
         <v>136</v>
       </c>
-      <c r="AP7" s="21" t="s">
+      <c r="AQ7" s="21" t="s">
         <v>137</v>
       </c>
-      <c r="AQ7" s="22" t="s">
+      <c r="AR7" s="22" t="s">
         <v>206</v>
       </c>
-      <c r="AR7" s="22" t="s">
+      <c r="AS7" s="22" t="s">
         <v>207</v>
       </c>
-      <c r="AS7" s="22" t="s">
+      <c r="AT7" s="22" t="s">
         <v>208</v>
       </c>
-      <c r="AT7" s="6" t="s">
+      <c r="AU7" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="AU7" s="2" t="s">
+      <c r="AV7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="AV7" s="2" t="s">
+      <c r="AW7" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="AW7" s="2" t="s">
+      <c r="AX7" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="AX7" s="2" t="s">
+      <c r="AY7" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="AY7" s="18" t="s">
+      <c r="AZ7" s="18" t="s">
         <v>202</v>
       </c>
-      <c r="AZ7" s="18" t="s">
+      <c r="BA7" s="18" t="s">
         <v>209</v>
       </c>
-      <c r="BA7" s="18" t="s">
+      <c r="BB7" s="18" t="s">
         <v>210</v>
       </c>
-      <c r="BB7" s="18" t="s">
+      <c r="BC7" s="18" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="8" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A8" s="19" t="s">
         <v>224</v>
       </c>
@@ -1501,8 +1508,8 @@
       <c r="D8" s="7"/>
       <c r="E8" s="7"/>
     </row>
-    <row r="9" spans="1:54" x14ac:dyDescent="0.25">
-      <c r="A9" s="26" t="s">
+    <row r="9" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="A9" s="25" t="s">
         <v>225</v>
       </c>
       <c r="B9" s="19"/>
@@ -1510,7 +1517,7 @@
       <c r="D9" s="7"/>
       <c r="E9" s="7"/>
     </row>
-    <row r="10" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A10" s="24" t="s">
         <v>226</v>
       </c>
@@ -1521,8 +1528,8 @@
       <c r="D10" s="7"/>
       <c r="E10" s="7"/>
     </row>
-    <row r="11" spans="1:54" x14ac:dyDescent="0.25">
-      <c r="A11" s="26" t="s">
+    <row r="11" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="A11" s="25" t="s">
         <v>227</v>
       </c>
       <c r="B11" s="19"/>
@@ -1532,7 +1539,7 @@
       <c r="D11" s="7"/>
       <c r="E11" s="7"/>
     </row>
-    <row r="12" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A12" s="24" t="s">
         <v>228</v>
       </c>
@@ -1543,8 +1550,8 @@
       <c r="D12" s="7"/>
       <c r="E12" s="7"/>
     </row>
-    <row r="13" spans="1:54" x14ac:dyDescent="0.25">
-      <c r="A13" s="26" t="s">
+    <row r="13" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="A13" s="25" t="s">
         <v>229</v>
       </c>
       <c r="B13" s="19"/>
@@ -1554,7 +1561,7 @@
       <c r="D13" s="7"/>
       <c r="E13" s="7"/>
     </row>
-    <row r="14" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A14" s="24" t="s">
         <v>230</v>
       </c>
@@ -1563,14 +1570,14 @@
       <c r="D14" s="7"/>
       <c r="E14" s="7"/>
     </row>
-    <row r="15" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A15" s="19"/>
       <c r="B15" s="19"/>
       <c r="C15" s="19"/>
       <c r="D15" s="7"/>
       <c r="E15" s="7"/>
     </row>
-    <row r="16" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A16" s="19"/>
       <c r="B16" s="19"/>
       <c r="C16" s="19"/>

</xml_diff>

<commit_message>
Added GIFs for README
</commit_message>
<xml_diff>
--- a/GetInventory - Default.xlsx
+++ b/GetInventory - Default.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PycharmProjects\GetInventory\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31C451E7-E9CA-40B0-B442-F2DBD06FEAB5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66EBFEA4-C158-4091-A023-51841AE1ED66}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20700" yWindow="3110" windowWidth="17270" windowHeight="10780" tabRatio="849" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="450" yWindow="760" windowWidth="15960" windowHeight="10800" tabRatio="849" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="227">
   <si>
     <t>Username</t>
   </si>
@@ -708,10 +708,31 @@
     <t>https://github.com/tc45/GetInventory</t>
   </si>
   <si>
-    <t>c:\temp\GetInventory\Customer\Project</t>
-  </si>
-  <si>
-    <t>Site1</t>
+    <t>myusername</t>
+  </si>
+  <si>
+    <t>mypassword</t>
+  </si>
+  <si>
+    <t>mysecret</t>
+  </si>
+  <si>
+    <t>c:\temp\GetInventory\XYZ_Corporation\Network Discovery</t>
+  </si>
+  <si>
+    <t>NYC-1</t>
+  </si>
+  <si>
+    <t>10.1.1.1</t>
+  </si>
+  <si>
+    <t>10.1.1.2</t>
+  </si>
+  <si>
+    <t>10.1.1.3</t>
+  </si>
+  <si>
+    <t>10.1.1.4</t>
   </si>
 </sst>
 </file>
@@ -1463,7 +1484,9 @@
   </sheetPr>
   <dimension ref="A1:BC68"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -1500,7 +1523,9 @@
       <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22"/>
+      <c r="B1" s="22" t="s">
+        <v>218</v>
+      </c>
       <c r="C1" s="22"/>
       <c r="D1" s="22"/>
       <c r="E1" s="22"/>
@@ -1515,7 +1540,9 @@
       <c r="A2" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="24"/>
+      <c r="B2" s="24" t="s">
+        <v>219</v>
+      </c>
       <c r="C2" s="24"/>
       <c r="D2" s="24"/>
       <c r="E2" s="24"/>
@@ -1530,7 +1557,9 @@
       <c r="A3" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="24"/>
+      <c r="B3" s="24" t="s">
+        <v>220</v>
+      </c>
       <c r="C3" s="24"/>
       <c r="D3" s="24"/>
       <c r="E3" s="24"/>
@@ -1544,7 +1573,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="26" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="C4" s="26"/>
       <c r="D4" s="26"/>
@@ -1557,7 +1586,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="28" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="C5" s="28"/>
       <c r="D5" s="28"/>
@@ -1733,8 +1762,25 @@
         <v>205</v>
       </c>
     </row>
+    <row r="8" spans="1:55" x14ac:dyDescent="0.35">
+      <c r="A8" s="12" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="9" spans="1:55" x14ac:dyDescent="0.35">
+      <c r="A9" s="12" t="s">
+        <v>224</v>
+      </c>
+    </row>
     <row r="10" spans="1:55" x14ac:dyDescent="0.35">
-      <c r="A10" s="13"/>
+      <c r="A10" s="13" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="11" spans="1:55" x14ac:dyDescent="0.35">
+      <c r="A11" s="12" t="s">
+        <v>226</v>
+      </c>
     </row>
     <row r="12" spans="1:55" x14ac:dyDescent="0.35">
       <c r="A12" s="13"/>
@@ -1952,7 +1998,7 @@
     <mergeCell ref="B5:G5"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
-  <dataValidations disablePrompts="1" count="5">
+  <dataValidations count="5">
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B991:B1225 D8:D14" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"ssh, telnet"</formula1>
     </dataValidation>

</xml_diff>

<commit_message>
Reverting back to earlier version
</commit_message>
<xml_diff>
--- a/GetInventory - Default.xlsx
+++ b/GetInventory - Default.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Python\GetInventory\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PycharmProjects\GetInventory\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48D09F1B-24D2-4A17-B894-D808CF61C499}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C0F67E2-A4C2-43F7-A57B-AD49B3D4BE2B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" tabRatio="849" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4250" yWindow="6070" windowWidth="15840" windowHeight="9470" tabRatio="849" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -570,9 +570,6 @@
     <t>c:\temp\GetInventory\XYZ_CORP\Project_X</t>
   </si>
   <si>
-    <t>Site_NYC-1</t>
-  </si>
-  <si>
     <t xml:space="preserve">Below are the settings for the behavior of this application. Toggle the features to No to turn the features off.  </t>
   </si>
   <si>
@@ -589,6 +586,9 @@
   </si>
   <si>
     <t>https://github.com/tc45/GetInventory</t>
+  </si>
+  <si>
+    <t>Site_1</t>
   </si>
 </sst>
 </file>
@@ -910,21 +910,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0" hidden="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="8" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0" hidden="1"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
@@ -942,29 +940,31 @@
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -1308,7 +1308,7 @@
   <dimension ref="A1:AZ14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1343,21 +1343,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:52" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="21"/>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="33"/>
       <c r="H1" s="17"/>
       <c r="I1" s="17"/>
-      <c r="J1" s="33" t="s">
-        <v>177</v>
-      </c>
-      <c r="K1" s="33"/>
+      <c r="J1" s="30" t="s">
+        <v>176</v>
+      </c>
+      <c r="K1" s="30"/>
       <c r="L1" s="17"/>
       <c r="M1" s="17"/>
       <c r="N1" s="17"/>
@@ -1401,21 +1401,21 @@
       <c r="AZ1" s="17"/>
     </row>
     <row r="2" spans="1:52" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="22"/>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="23"/>
+      <c r="B2" s="35"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="36"/>
       <c r="H2" s="17"/>
       <c r="I2" s="17"/>
-      <c r="J2" s="32" t="s">
-        <v>178</v>
-      </c>
-      <c r="K2" s="32"/>
+      <c r="J2" s="31" t="s">
+        <v>177</v>
+      </c>
+      <c r="K2" s="31"/>
       <c r="L2" s="17"/>
       <c r="M2" s="17"/>
       <c r="N2" s="17"/>
@@ -1459,15 +1459,15 @@
       <c r="AZ2" s="17"/>
     </row>
     <row r="3" spans="1:52" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A3" s="35" t="s">
+      <c r="A3" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="22"/>
-      <c r="C3" s="22"/>
-      <c r="D3" s="22"/>
-      <c r="E3" s="22"/>
-      <c r="F3" s="22"/>
-      <c r="G3" s="23"/>
+      <c r="B3" s="35"/>
+      <c r="C3" s="35"/>
+      <c r="D3" s="35"/>
+      <c r="E3" s="35"/>
+      <c r="F3" s="35"/>
+      <c r="G3" s="36"/>
       <c r="H3" s="17"/>
       <c r="I3" s="17"/>
       <c r="J3" s="17"/>
@@ -1515,17 +1515,17 @@
       <c r="AZ3" s="17"/>
     </row>
     <row r="4" spans="1:52" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="35" t="s">
+      <c r="A4" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="24" t="s">
+      <c r="B4" s="26" t="s">
         <v>171</v>
       </c>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="24"/>
-      <c r="G4" s="25"/>
+      <c r="C4" s="26"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="26"/>
+      <c r="F4" s="26"/>
+      <c r="G4" s="27"/>
       <c r="H4" s="17"/>
       <c r="I4" s="17"/>
       <c r="J4" s="17"/>
@@ -1573,17 +1573,17 @@
       <c r="AZ4" s="17"/>
     </row>
     <row r="5" spans="1:52" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="36" t="s">
+      <c r="A5" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="26" t="s">
-        <v>172</v>
-      </c>
-      <c r="C5" s="26"/>
-      <c r="D5" s="26"/>
-      <c r="E5" s="26"/>
-      <c r="F5" s="26"/>
-      <c r="G5" s="27"/>
+      <c r="B5" s="28" t="s">
+        <v>178</v>
+      </c>
+      <c r="C5" s="28"/>
+      <c r="D5" s="28"/>
+      <c r="E5" s="28"/>
+      <c r="F5" s="28"/>
+      <c r="G5" s="29"/>
       <c r="H5" s="17"/>
       <c r="I5" s="17"/>
       <c r="J5" s="17"/>
@@ -1852,18 +1852,18 @@
       <c r="A14" s="19"/>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1" formatCells="0" formatColumns="0" formatRows="0"/>
+  <sheetProtection formatCells="0" formatColumns="0" formatRows="0"/>
   <mergeCells count="7">
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="B5:G5"/>
     <mergeCell ref="J1:K1"/>
     <mergeCell ref="J2:K2"/>
     <mergeCell ref="B1:G1"/>
     <mergeCell ref="B2:G2"/>
     <mergeCell ref="B3:G3"/>
-    <mergeCell ref="B4:G4"/>
-    <mergeCell ref="B5:G5"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
-  <dataValidations count="5">
+  <dataValidations disablePrompts="1" count="5">
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B991:B1225 D8:D14" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"ssh, telnet"</formula1>
     </dataValidation>
@@ -2068,36 +2068,36 @@
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="19.81640625" style="3" hidden="1" customWidth="1"/>
-    <col min="2" max="2" width="30.7265625" style="28" customWidth="1"/>
-    <col min="3" max="3" width="19.81640625" style="28" customWidth="1"/>
-    <col min="4" max="16384" width="9.1796875" style="28"/>
+    <col min="2" max="2" width="30.7265625" style="20" customWidth="1"/>
+    <col min="3" max="3" width="19.81640625" style="20" customWidth="1"/>
+    <col min="4" max="16384" width="9.1796875" style="20"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="31" x14ac:dyDescent="0.7">
-      <c r="B1" s="31" t="s">
-        <v>176</v>
+      <c r="B1" s="22" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="10"/>
-      <c r="B2" s="30" t="s">
-        <v>173</v>
-      </c>
-      <c r="C2" s="30"/>
+      <c r="B2" s="34" t="s">
+        <v>172</v>
+      </c>
+      <c r="C2" s="34"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B3" s="29"/>
-      <c r="C3" s="29"/>
+      <c r="B3" s="21"/>
+      <c r="C3" s="21"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>136</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>174</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Reset to 11/5/2020 commit prior to overhaul.
</commit_message>
<xml_diff>
--- a/GetInventory - Default.xlsx
+++ b/GetInventory - Default.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://insightonline-my.sharepoint.com/personal/ruben_gutierrezmartinez_insight_com/Documents/Documents/GitHub/GetInventory/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tony\PycharmProjects\GetInventory\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="12" documentId="13_ncr:1_{3BF8DEBB-66D5-4598-82DF-D5459BDD8E12}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{3DAEDAF1-643A-4BA0-A2F9-24005E5BF250}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0026881B-9ACD-4537-89A5-C324CBBD0D00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="849" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6840" yWindow="1840" windowWidth="28800" windowHeight="15460" tabRatio="849" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="186">
   <si>
     <t>Username</t>
   </si>
@@ -595,6 +595,21 @@
   </si>
   <si>
     <t>Elapsed Time (Seconds)</t>
+  </si>
+  <si>
+    <t>192.168.1.192</t>
+  </si>
+  <si>
+    <t>10.1.1.1</t>
+  </si>
+  <si>
+    <t>cisco_ios</t>
+  </si>
+  <si>
+    <t>autodetect</t>
+  </si>
+  <si>
+    <t>cisco</t>
   </si>
 </sst>
 </file>
@@ -859,23 +874,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment textRotation="60"/>
       <protection locked="0"/>
@@ -900,9 +906,6 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
@@ -1303,560 +1306,579 @@
   <sheetPr>
     <tabColor theme="5" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="A1:BA14"/>
+  <dimension ref="A1:BA9"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20.44140625" style="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.77734375" style="16" customWidth="1"/>
-    <col min="3" max="3" width="11.21875" style="16" customWidth="1"/>
-    <col min="4" max="4" width="8.77734375" style="16" customWidth="1"/>
-    <col min="5" max="5" width="7" style="16" customWidth="1"/>
-    <col min="6" max="6" width="14.21875" style="16" customWidth="1"/>
-    <col min="7" max="7" width="13.5546875" style="16" customWidth="1"/>
-    <col min="8" max="8" width="20.5546875" style="16" customWidth="1"/>
-    <col min="9" max="9" width="10.77734375" style="16" customWidth="1"/>
-    <col min="10" max="10" width="25.21875" style="16" customWidth="1"/>
-    <col min="11" max="11" width="16.5546875" style="16" customWidth="1"/>
-    <col min="12" max="12" width="15.44140625" style="16" customWidth="1"/>
-    <col min="13" max="13" width="8.77734375" style="16"/>
-    <col min="14" max="14" width="16" style="16" customWidth="1"/>
-    <col min="15" max="15" width="20" style="16" customWidth="1"/>
-    <col min="16" max="16" width="16" style="16" customWidth="1"/>
-    <col min="17" max="17" width="51.21875" style="16" customWidth="1"/>
-    <col min="18" max="34" width="4.21875" style="16" customWidth="1"/>
-    <col min="35" max="45" width="4.44140625" style="16" customWidth="1"/>
-    <col min="46" max="47" width="8.77734375" style="16"/>
-    <col min="48" max="48" width="16.77734375" style="16" customWidth="1"/>
-    <col min="49" max="49" width="74.21875" style="16" customWidth="1"/>
-    <col min="50" max="50" width="54.5546875" style="16" customWidth="1"/>
-    <col min="51" max="51" width="37.21875" style="16" customWidth="1"/>
-    <col min="52" max="52" width="37.77734375" style="16" customWidth="1"/>
-    <col min="53" max="53" width="8.77734375" style="16"/>
-    <col min="54" max="16384" width="8.77734375" style="15"/>
+    <col min="1" max="1" width="20.453125" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.81640625" style="9" customWidth="1"/>
+    <col min="3" max="3" width="11.1796875" style="9" customWidth="1"/>
+    <col min="4" max="4" width="8.81640625" style="9" customWidth="1"/>
+    <col min="5" max="5" width="7" style="9" customWidth="1"/>
+    <col min="6" max="6" width="14.1796875" style="9" customWidth="1"/>
+    <col min="7" max="7" width="13.54296875" style="9" customWidth="1"/>
+    <col min="8" max="8" width="20.54296875" style="9" customWidth="1"/>
+    <col min="9" max="9" width="10.81640625" style="9" customWidth="1"/>
+    <col min="10" max="10" width="25.1796875" style="9" customWidth="1"/>
+    <col min="11" max="11" width="16.54296875" style="9" customWidth="1"/>
+    <col min="12" max="12" width="15.453125" style="9" customWidth="1"/>
+    <col min="13" max="13" width="8.81640625" style="9"/>
+    <col min="14" max="14" width="16" style="9" customWidth="1"/>
+    <col min="15" max="15" width="20" style="9" customWidth="1"/>
+    <col min="16" max="16" width="16" style="9" customWidth="1"/>
+    <col min="17" max="17" width="51.1796875" style="9" customWidth="1"/>
+    <col min="18" max="34" width="4.1796875" style="9" customWidth="1"/>
+    <col min="35" max="45" width="4.453125" style="9" customWidth="1"/>
+    <col min="46" max="47" width="8.81640625" style="9"/>
+    <col min="48" max="48" width="16.81640625" style="9" customWidth="1"/>
+    <col min="49" max="49" width="74.1796875" style="9" customWidth="1"/>
+    <col min="50" max="50" width="54.54296875" style="9" customWidth="1"/>
+    <col min="51" max="51" width="37.1796875" style="9" customWidth="1"/>
+    <col min="52" max="52" width="37.81640625" style="9" customWidth="1"/>
+    <col min="53" max="53" width="8.81640625" style="9"/>
+    <col min="54" max="16384" width="8.81640625" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:53" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="19" t="s">
+    <row r="1" spans="1:53" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="28" t="s">
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="20" t="s">
         <v>172</v>
       </c>
-      <c r="K1" s="28"/>
-      <c r="L1" s="15"/>
-      <c r="M1" s="15"/>
-      <c r="N1" s="15"/>
-      <c r="O1" s="15"/>
-      <c r="P1" s="15"/>
-      <c r="Q1" s="15"/>
-      <c r="R1" s="15"/>
-      <c r="S1" s="15"/>
-      <c r="T1" s="15"/>
-      <c r="U1" s="15"/>
-      <c r="V1" s="15"/>
-      <c r="W1" s="15"/>
-      <c r="X1" s="15"/>
-      <c r="Y1" s="15"/>
-      <c r="Z1" s="15"/>
-      <c r="AA1" s="15"/>
-      <c r="AB1" s="15"/>
-      <c r="AC1" s="15"/>
-      <c r="AD1" s="15"/>
-      <c r="AE1" s="15"/>
-      <c r="AF1" s="15"/>
-      <c r="AG1" s="15"/>
-      <c r="AH1" s="15"/>
-      <c r="AI1" s="15"/>
-      <c r="AJ1" s="15"/>
-      <c r="AK1" s="15"/>
-      <c r="AL1" s="15"/>
-      <c r="AM1" s="15"/>
-      <c r="AN1" s="15"/>
-      <c r="AO1" s="15"/>
-      <c r="AP1" s="15"/>
-      <c r="AQ1" s="15"/>
-      <c r="AR1" s="15"/>
-      <c r="AS1" s="15"/>
-      <c r="AT1" s="15"/>
-      <c r="AU1" s="15"/>
-      <c r="AV1" s="15"/>
-      <c r="AW1" s="15"/>
-      <c r="AX1" s="15"/>
-      <c r="AY1" s="15"/>
-      <c r="AZ1" s="15"/>
-      <c r="BA1" s="15"/>
-    </row>
-    <row r="2" spans="1:53" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="20" t="s">
+      <c r="K1" s="20"/>
+      <c r="L1" s="8"/>
+      <c r="M1" s="8"/>
+      <c r="N1" s="8"/>
+      <c r="O1" s="8"/>
+      <c r="P1" s="8"/>
+      <c r="Q1" s="8"/>
+      <c r="R1" s="8"/>
+      <c r="S1" s="8"/>
+      <c r="T1" s="8"/>
+      <c r="U1" s="8"/>
+      <c r="V1" s="8"/>
+      <c r="W1" s="8"/>
+      <c r="X1" s="8"/>
+      <c r="Y1" s="8"/>
+      <c r="Z1" s="8"/>
+      <c r="AA1" s="8"/>
+      <c r="AB1" s="8"/>
+      <c r="AC1" s="8"/>
+      <c r="AD1" s="8"/>
+      <c r="AE1" s="8"/>
+      <c r="AF1" s="8"/>
+      <c r="AG1" s="8"/>
+      <c r="AH1" s="8"/>
+      <c r="AI1" s="8"/>
+      <c r="AJ1" s="8"/>
+      <c r="AK1" s="8"/>
+      <c r="AL1" s="8"/>
+      <c r="AM1" s="8"/>
+      <c r="AN1" s="8"/>
+      <c r="AO1" s="8"/>
+      <c r="AP1" s="8"/>
+      <c r="AQ1" s="8"/>
+      <c r="AR1" s="8"/>
+      <c r="AS1" s="8"/>
+      <c r="AT1" s="8"/>
+      <c r="AU1" s="8"/>
+      <c r="AV1" s="8"/>
+      <c r="AW1" s="8"/>
+      <c r="AX1" s="8"/>
+      <c r="AY1" s="8"/>
+      <c r="AZ1" s="8"/>
+      <c r="BA1" s="8"/>
+    </row>
+    <row r="2" spans="1:53" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A2" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="33"/>
-      <c r="H2" s="15"/>
-      <c r="I2" s="15"/>
-      <c r="J2" s="29" t="s">
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="21" t="s">
         <v>173</v>
       </c>
-      <c r="K2" s="29"/>
-      <c r="L2" s="15"/>
-      <c r="M2" s="15"/>
-      <c r="N2" s="15"/>
-      <c r="O2" s="15"/>
-      <c r="P2" s="15"/>
-      <c r="Q2" s="15"/>
-      <c r="R2" s="15"/>
-      <c r="S2" s="15"/>
-      <c r="T2" s="15"/>
-      <c r="U2" s="15"/>
-      <c r="V2" s="15"/>
-      <c r="W2" s="15"/>
-      <c r="X2" s="15"/>
-      <c r="Y2" s="15"/>
-      <c r="Z2" s="15"/>
-      <c r="AA2" s="15"/>
-      <c r="AB2" s="15"/>
-      <c r="AC2" s="15"/>
-      <c r="AD2" s="15"/>
-      <c r="AE2" s="15"/>
-      <c r="AF2" s="15"/>
-      <c r="AG2" s="15"/>
-      <c r="AH2" s="15"/>
-      <c r="AI2" s="15"/>
-      <c r="AJ2" s="15"/>
-      <c r="AK2" s="15"/>
-      <c r="AL2" s="15"/>
-      <c r="AM2" s="15"/>
-      <c r="AN2" s="15"/>
-      <c r="AO2" s="15"/>
-      <c r="AP2" s="15"/>
-      <c r="AQ2" s="15"/>
-      <c r="AR2" s="15"/>
-      <c r="AS2" s="15"/>
-      <c r="AT2" s="15"/>
-      <c r="AU2" s="15"/>
-      <c r="AV2" s="15"/>
-      <c r="AW2" s="15"/>
-      <c r="AX2" s="15"/>
-      <c r="AY2" s="15"/>
-      <c r="AZ2" s="15"/>
-      <c r="BA2" s="15"/>
-    </row>
-    <row r="3" spans="1:53" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A3" s="20" t="s">
+      <c r="K2" s="21"/>
+      <c r="L2" s="8"/>
+      <c r="M2" s="8"/>
+      <c r="N2" s="8"/>
+      <c r="O2" s="8"/>
+      <c r="P2" s="8"/>
+      <c r="Q2" s="8"/>
+      <c r="R2" s="8"/>
+      <c r="S2" s="8"/>
+      <c r="T2" s="8"/>
+      <c r="U2" s="8"/>
+      <c r="V2" s="8"/>
+      <c r="W2" s="8"/>
+      <c r="X2" s="8"/>
+      <c r="Y2" s="8"/>
+      <c r="Z2" s="8"/>
+      <c r="AA2" s="8"/>
+      <c r="AB2" s="8"/>
+      <c r="AC2" s="8"/>
+      <c r="AD2" s="8"/>
+      <c r="AE2" s="8"/>
+      <c r="AF2" s="8"/>
+      <c r="AG2" s="8"/>
+      <c r="AH2" s="8"/>
+      <c r="AI2" s="8"/>
+      <c r="AJ2" s="8"/>
+      <c r="AK2" s="8"/>
+      <c r="AL2" s="8"/>
+      <c r="AM2" s="8"/>
+      <c r="AN2" s="8"/>
+      <c r="AO2" s="8"/>
+      <c r="AP2" s="8"/>
+      <c r="AQ2" s="8"/>
+      <c r="AR2" s="8"/>
+      <c r="AS2" s="8"/>
+      <c r="AT2" s="8"/>
+      <c r="AU2" s="8"/>
+      <c r="AV2" s="8"/>
+      <c r="AW2" s="8"/>
+      <c r="AX2" s="8"/>
+      <c r="AY2" s="8"/>
+      <c r="AZ2" s="8"/>
+      <c r="BA2" s="8"/>
+    </row>
+    <row r="3" spans="1:53" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A3" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="32"/>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="32"/>
-      <c r="G3" s="33"/>
-      <c r="H3" s="15"/>
-      <c r="I3" s="15"/>
-      <c r="J3" s="15"/>
-      <c r="K3" s="15"/>
-      <c r="L3" s="15"/>
-      <c r="M3" s="15"/>
-      <c r="N3" s="15"/>
-      <c r="O3" s="15"/>
-      <c r="P3" s="15"/>
-      <c r="Q3" s="15"/>
-      <c r="R3" s="15"/>
-      <c r="S3" s="15"/>
-      <c r="T3" s="15"/>
-      <c r="U3" s="15"/>
-      <c r="V3" s="15"/>
-      <c r="W3" s="15"/>
-      <c r="X3" s="15"/>
-      <c r="Y3" s="15"/>
-      <c r="Z3" s="15"/>
-      <c r="AA3" s="15"/>
-      <c r="AB3" s="15"/>
-      <c r="AC3" s="15"/>
-      <c r="AD3" s="15"/>
-      <c r="AE3" s="15"/>
-      <c r="AF3" s="15"/>
-      <c r="AG3" s="15"/>
-      <c r="AH3" s="15"/>
-      <c r="AI3" s="15"/>
-      <c r="AJ3" s="15"/>
-      <c r="AK3" s="15"/>
-      <c r="AL3" s="15"/>
-      <c r="AM3" s="15"/>
-      <c r="AN3" s="15"/>
-      <c r="AO3" s="15"/>
-      <c r="AP3" s="15"/>
-      <c r="AQ3" s="15"/>
-      <c r="AR3" s="15"/>
-      <c r="AS3" s="15"/>
-      <c r="AT3" s="15"/>
-      <c r="AU3" s="15"/>
-      <c r="AV3" s="15"/>
-      <c r="AW3" s="15"/>
-      <c r="AX3" s="15"/>
-      <c r="AY3" s="15"/>
-      <c r="AZ3" s="15"/>
-      <c r="BA3" s="15"/>
-    </row>
-    <row r="4" spans="1:53" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="20" t="s">
+      <c r="B3" s="24"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="8"/>
+      <c r="L3" s="8"/>
+      <c r="M3" s="8"/>
+      <c r="N3" s="8"/>
+      <c r="O3" s="8"/>
+      <c r="P3" s="8"/>
+      <c r="Q3" s="8"/>
+      <c r="R3" s="8"/>
+      <c r="S3" s="8"/>
+      <c r="T3" s="8"/>
+      <c r="U3" s="8"/>
+      <c r="V3" s="8"/>
+      <c r="W3" s="8"/>
+      <c r="X3" s="8"/>
+      <c r="Y3" s="8"/>
+      <c r="Z3" s="8"/>
+      <c r="AA3" s="8"/>
+      <c r="AB3" s="8"/>
+      <c r="AC3" s="8"/>
+      <c r="AD3" s="8"/>
+      <c r="AE3" s="8"/>
+      <c r="AF3" s="8"/>
+      <c r="AG3" s="8"/>
+      <c r="AH3" s="8"/>
+      <c r="AI3" s="8"/>
+      <c r="AJ3" s="8"/>
+      <c r="AK3" s="8"/>
+      <c r="AL3" s="8"/>
+      <c r="AM3" s="8"/>
+      <c r="AN3" s="8"/>
+      <c r="AO3" s="8"/>
+      <c r="AP3" s="8"/>
+      <c r="AQ3" s="8"/>
+      <c r="AR3" s="8"/>
+      <c r="AS3" s="8"/>
+      <c r="AT3" s="8"/>
+      <c r="AU3" s="8"/>
+      <c r="AV3" s="8"/>
+      <c r="AW3" s="8"/>
+      <c r="AX3" s="8"/>
+      <c r="AY3" s="8"/>
+      <c r="AZ3" s="8"/>
+      <c r="BA3" s="8"/>
+    </row>
+    <row r="4" spans="1:53" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A4" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="24" t="s">
+      <c r="B4" s="16" t="s">
         <v>169</v>
       </c>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="24"/>
-      <c r="G4" s="25"/>
-      <c r="H4" s="15"/>
-      <c r="I4" s="15"/>
-      <c r="J4" s="15"/>
-      <c r="K4" s="15"/>
-      <c r="L4" s="15"/>
-      <c r="M4" s="15"/>
-      <c r="N4" s="15"/>
-      <c r="O4" s="15"/>
-      <c r="P4" s="15"/>
-      <c r="Q4" s="15"/>
-      <c r="R4" s="15"/>
-      <c r="S4" s="15"/>
-      <c r="T4" s="15"/>
-      <c r="U4" s="15"/>
-      <c r="V4" s="15"/>
-      <c r="W4" s="15"/>
-      <c r="X4" s="15"/>
-      <c r="Y4" s="15"/>
-      <c r="Z4" s="15"/>
-      <c r="AA4" s="15"/>
-      <c r="AB4" s="15"/>
-      <c r="AC4" s="15"/>
-      <c r="AD4" s="15"/>
-      <c r="AE4" s="15"/>
-      <c r="AF4" s="15"/>
-      <c r="AG4" s="15"/>
-      <c r="AH4" s="15"/>
-      <c r="AI4" s="15"/>
-      <c r="AJ4" s="15"/>
-      <c r="AK4" s="15"/>
-      <c r="AL4" s="15"/>
-      <c r="AM4" s="15"/>
-      <c r="AN4" s="15"/>
-      <c r="AO4" s="15"/>
-      <c r="AP4" s="15"/>
-      <c r="AQ4" s="15"/>
-      <c r="AR4" s="15"/>
-      <c r="AS4" s="15"/>
-      <c r="AT4" s="15"/>
-      <c r="AU4" s="15"/>
-      <c r="AV4" s="15"/>
-      <c r="AW4" s="15"/>
-      <c r="AX4" s="15"/>
-      <c r="AY4" s="15"/>
-      <c r="AZ4" s="15"/>
-      <c r="BA4" s="15"/>
-    </row>
-    <row r="5" spans="1:53" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="21" t="s">
+      <c r="C4" s="16"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="16"/>
+      <c r="F4" s="16"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8"/>
+      <c r="J4" s="8"/>
+      <c r="K4" s="8"/>
+      <c r="L4" s="8"/>
+      <c r="M4" s="8"/>
+      <c r="N4" s="8"/>
+      <c r="O4" s="8"/>
+      <c r="P4" s="8"/>
+      <c r="Q4" s="8"/>
+      <c r="R4" s="8"/>
+      <c r="S4" s="8"/>
+      <c r="T4" s="8"/>
+      <c r="U4" s="8"/>
+      <c r="V4" s="8"/>
+      <c r="W4" s="8"/>
+      <c r="X4" s="8"/>
+      <c r="Y4" s="8"/>
+      <c r="Z4" s="8"/>
+      <c r="AA4" s="8"/>
+      <c r="AB4" s="8"/>
+      <c r="AC4" s="8"/>
+      <c r="AD4" s="8"/>
+      <c r="AE4" s="8"/>
+      <c r="AF4" s="8"/>
+      <c r="AG4" s="8"/>
+      <c r="AH4" s="8"/>
+      <c r="AI4" s="8"/>
+      <c r="AJ4" s="8"/>
+      <c r="AK4" s="8"/>
+      <c r="AL4" s="8"/>
+      <c r="AM4" s="8"/>
+      <c r="AN4" s="8"/>
+      <c r="AO4" s="8"/>
+      <c r="AP4" s="8"/>
+      <c r="AQ4" s="8"/>
+      <c r="AR4" s="8"/>
+      <c r="AS4" s="8"/>
+      <c r="AT4" s="8"/>
+      <c r="AU4" s="8"/>
+      <c r="AV4" s="8"/>
+      <c r="AW4" s="8"/>
+      <c r="AX4" s="8"/>
+      <c r="AY4" s="8"/>
+      <c r="AZ4" s="8"/>
+      <c r="BA4" s="8"/>
+    </row>
+    <row r="5" spans="1:53" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="26" t="s">
+      <c r="B5" s="18" t="s">
         <v>174</v>
       </c>
-      <c r="C5" s="26"/>
-      <c r="D5" s="26"/>
-      <c r="E5" s="26"/>
-      <c r="F5" s="26"/>
-      <c r="G5" s="27"/>
-      <c r="H5" s="15"/>
-      <c r="I5" s="15"/>
-      <c r="J5" s="15"/>
-      <c r="K5" s="15"/>
-      <c r="L5" s="15"/>
-      <c r="M5" s="15"/>
-      <c r="N5" s="15"/>
-      <c r="O5" s="15"/>
-      <c r="P5" s="15"/>
-      <c r="Q5" s="15"/>
-      <c r="R5" s="15"/>
-      <c r="S5" s="15"/>
-      <c r="T5" s="15"/>
-      <c r="U5" s="15"/>
-      <c r="V5" s="15"/>
-      <c r="W5" s="15"/>
-      <c r="X5" s="15"/>
-      <c r="Y5" s="15"/>
-      <c r="Z5" s="15"/>
-      <c r="AA5" s="15"/>
-      <c r="AB5" s="15"/>
-      <c r="AC5" s="15"/>
-      <c r="AD5" s="15"/>
-      <c r="AE5" s="15"/>
-      <c r="AF5" s="15"/>
-      <c r="AG5" s="15"/>
-      <c r="AH5" s="15"/>
-      <c r="AI5" s="15"/>
-      <c r="AJ5" s="15"/>
-      <c r="AK5" s="15"/>
-      <c r="AL5" s="15"/>
-      <c r="AM5" s="15"/>
-      <c r="AN5" s="15"/>
-      <c r="AO5" s="15"/>
-      <c r="AP5" s="15"/>
-      <c r="AQ5" s="15"/>
-      <c r="AR5" s="15"/>
-      <c r="AS5" s="15"/>
-      <c r="AT5" s="15"/>
-      <c r="AU5" s="15"/>
-      <c r="AV5" s="15"/>
-      <c r="AW5" s="15"/>
-      <c r="AX5" s="15"/>
-      <c r="AY5" s="15"/>
-      <c r="AZ5" s="15"/>
-      <c r="BA5" s="15"/>
-    </row>
-    <row r="6" spans="1:53" x14ac:dyDescent="0.3">
-      <c r="A6" s="15"/>
-      <c r="B6" s="15"/>
-      <c r="C6" s="15"/>
-      <c r="D6" s="15"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="15"/>
-      <c r="G6" s="15"/>
-      <c r="H6" s="15"/>
-      <c r="I6" s="15"/>
-      <c r="J6" s="15"/>
-      <c r="K6" s="15"/>
-      <c r="L6" s="15"/>
-      <c r="M6" s="15"/>
-      <c r="N6" s="15"/>
-      <c r="O6" s="15"/>
-      <c r="P6" s="15"/>
-      <c r="Q6" s="15"/>
-      <c r="R6" s="15"/>
-      <c r="S6" s="15"/>
-      <c r="T6" s="15"/>
-      <c r="U6" s="15"/>
-      <c r="V6" s="15"/>
-      <c r="W6" s="15"/>
-      <c r="X6" s="15"/>
-      <c r="Y6" s="15"/>
-      <c r="Z6" s="15"/>
-      <c r="AA6" s="15"/>
-      <c r="AB6" s="15"/>
-      <c r="AC6" s="15"/>
-      <c r="AD6" s="15"/>
-      <c r="AE6" s="15"/>
-      <c r="AF6" s="15"/>
-      <c r="AG6" s="15"/>
-      <c r="AH6" s="15"/>
-      <c r="AI6" s="15"/>
-      <c r="AJ6" s="15"/>
-      <c r="AK6" s="15"/>
-      <c r="AL6" s="15"/>
-      <c r="AM6" s="15"/>
-      <c r="AN6" s="15"/>
-      <c r="AO6" s="15"/>
-      <c r="AP6" s="15"/>
-      <c r="AQ6" s="15"/>
-      <c r="AR6" s="15"/>
-      <c r="AS6" s="15"/>
-      <c r="AT6" s="15"/>
-      <c r="AU6" s="15"/>
-      <c r="AV6" s="15"/>
-      <c r="AW6" s="15"/>
-      <c r="AX6" s="15"/>
-      <c r="AY6" s="15"/>
-      <c r="AZ6" s="15"/>
-      <c r="BA6" s="15"/>
-    </row>
-    <row r="7" spans="1:53" ht="109.2" x14ac:dyDescent="0.3">
-      <c r="A7" s="10" t="s">
+      <c r="C5" s="18"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="18"/>
+      <c r="G5" s="19"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="8"/>
+      <c r="K5" s="8"/>
+      <c r="L5" s="8"/>
+      <c r="M5" s="8"/>
+      <c r="N5" s="8"/>
+      <c r="O5" s="8"/>
+      <c r="P5" s="8"/>
+      <c r="Q5" s="8"/>
+      <c r="R5" s="8"/>
+      <c r="S5" s="8"/>
+      <c r="T5" s="8"/>
+      <c r="U5" s="8"/>
+      <c r="V5" s="8"/>
+      <c r="W5" s="8"/>
+      <c r="X5" s="8"/>
+      <c r="Y5" s="8"/>
+      <c r="Z5" s="8"/>
+      <c r="AA5" s="8"/>
+      <c r="AB5" s="8"/>
+      <c r="AC5" s="8"/>
+      <c r="AD5" s="8"/>
+      <c r="AE5" s="8"/>
+      <c r="AF5" s="8"/>
+      <c r="AG5" s="8"/>
+      <c r="AH5" s="8"/>
+      <c r="AI5" s="8"/>
+      <c r="AJ5" s="8"/>
+      <c r="AK5" s="8"/>
+      <c r="AL5" s="8"/>
+      <c r="AM5" s="8"/>
+      <c r="AN5" s="8"/>
+      <c r="AO5" s="8"/>
+      <c r="AP5" s="8"/>
+      <c r="AQ5" s="8"/>
+      <c r="AR5" s="8"/>
+      <c r="AS5" s="8"/>
+      <c r="AT5" s="8"/>
+      <c r="AU5" s="8"/>
+      <c r="AV5" s="8"/>
+      <c r="AW5" s="8"/>
+      <c r="AX5" s="8"/>
+      <c r="AY5" s="8"/>
+      <c r="AZ5" s="8"/>
+      <c r="BA5" s="8"/>
+    </row>
+    <row r="6" spans="1:53" x14ac:dyDescent="0.35">
+      <c r="A6" s="8"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="8"/>
+      <c r="J6" s="8"/>
+      <c r="K6" s="8"/>
+      <c r="L6" s="8"/>
+      <c r="M6" s="8"/>
+      <c r="N6" s="8"/>
+      <c r="O6" s="8"/>
+      <c r="P6" s="8"/>
+      <c r="Q6" s="8"/>
+      <c r="R6" s="8"/>
+      <c r="S6" s="8"/>
+      <c r="T6" s="8"/>
+      <c r="U6" s="8"/>
+      <c r="V6" s="8"/>
+      <c r="W6" s="8"/>
+      <c r="X6" s="8"/>
+      <c r="Y6" s="8"/>
+      <c r="Z6" s="8"/>
+      <c r="AA6" s="8"/>
+      <c r="AB6" s="8"/>
+      <c r="AC6" s="8"/>
+      <c r="AD6" s="8"/>
+      <c r="AE6" s="8"/>
+      <c r="AF6" s="8"/>
+      <c r="AG6" s="8"/>
+      <c r="AH6" s="8"/>
+      <c r="AI6" s="8"/>
+      <c r="AJ6" s="8"/>
+      <c r="AK6" s="8"/>
+      <c r="AL6" s="8"/>
+      <c r="AM6" s="8"/>
+      <c r="AN6" s="8"/>
+      <c r="AO6" s="8"/>
+      <c r="AP6" s="8"/>
+      <c r="AQ6" s="8"/>
+      <c r="AR6" s="8"/>
+      <c r="AS6" s="8"/>
+      <c r="AT6" s="8"/>
+      <c r="AU6" s="8"/>
+      <c r="AV6" s="8"/>
+      <c r="AW6" s="8"/>
+      <c r="AX6" s="8"/>
+      <c r="AY6" s="8"/>
+      <c r="AZ6" s="8"/>
+      <c r="BA6" s="8"/>
+    </row>
+    <row r="7" spans="1:53" ht="108.5" x14ac:dyDescent="0.35">
+      <c r="A7" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="5" t="s">
         <v>152</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="D7" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E7" s="10" t="s">
+      <c r="E7" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F7" s="11" t="s">
+      <c r="F7" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="G7" s="11" t="s">
+      <c r="G7" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="H7" s="10" t="s">
+      <c r="H7" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="I7" s="10" t="s">
+      <c r="I7" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J7" s="10" t="s">
+      <c r="J7" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="K7" s="10" t="s">
+      <c r="K7" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="L7" s="10" t="s">
+      <c r="L7" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="M7" s="11" t="s">
+      <c r="M7" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="N7" s="11" t="s">
+      <c r="N7" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="O7" s="10" t="s">
+      <c r="O7" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="P7" s="10" t="s">
+      <c r="P7" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="Q7" s="10" t="s">
+      <c r="Q7" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="R7" s="13" t="s">
+      <c r="R7" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="S7" s="13" t="s">
+      <c r="S7" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="T7" s="13" t="s">
+      <c r="T7" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="U7" s="13" t="s">
+      <c r="U7" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="V7" s="13" t="s">
+      <c r="V7" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="W7" s="13" t="s">
+      <c r="W7" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="X7" s="13" t="s">
+      <c r="X7" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="Y7" s="13" t="s">
+      <c r="Y7" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="Z7" s="13" t="s">
+      <c r="Z7" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="AA7" s="13" t="s">
+      <c r="AA7" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="AB7" s="13" t="s">
+      <c r="AB7" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="AC7" s="13" t="s">
+      <c r="AC7" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="AD7" s="13" t="s">
+      <c r="AD7" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="AE7" s="13" t="s">
+      <c r="AE7" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="AF7" s="13" t="s">
+      <c r="AF7" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="AG7" s="13" t="s">
+      <c r="AG7" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="AH7" s="13" t="s">
+      <c r="AH7" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="AI7" s="13" t="s">
+      <c r="AI7" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="AJ7" s="13" t="s">
+      <c r="AJ7" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="AK7" s="13" t="s">
+      <c r="AK7" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="AL7" s="13" t="s">
+      <c r="AL7" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="AM7" s="13" t="s">
+      <c r="AM7" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="AN7" s="13" t="s">
+      <c r="AN7" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="AO7" s="13" t="s">
+      <c r="AO7" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="AP7" s="13" t="s">
+      <c r="AP7" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="AQ7" s="13" t="s">
+      <c r="AQ7" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="AR7" s="14" t="s">
+      <c r="AR7" s="7" t="s">
         <v>156</v>
       </c>
-      <c r="AS7" s="14" t="s">
+      <c r="AS7" s="7" t="s">
         <v>157</v>
       </c>
-      <c r="AT7" s="14" t="s">
+      <c r="AT7" s="7" t="s">
         <v>158</v>
       </c>
-      <c r="AU7" s="14" t="s">
+      <c r="AU7" s="7" t="s">
         <v>177</v>
       </c>
-      <c r="AV7" s="10" t="s">
+      <c r="AV7" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="AW7" s="10" t="s">
+      <c r="AW7" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="AX7" s="10" t="s">
+      <c r="AX7" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="AY7" s="10" t="s">
+      <c r="AY7" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="AZ7" s="10" t="s">
+      <c r="AZ7" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="BA7" s="10" t="s">
+      <c r="BA7" s="3" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="10" spans="1:53" x14ac:dyDescent="0.3">
-      <c r="A10" s="17"/>
-    </row>
-    <row r="12" spans="1:53" x14ac:dyDescent="0.3">
-      <c r="A12" s="17"/>
-    </row>
-    <row r="14" spans="1:53" x14ac:dyDescent="0.3">
-      <c r="A14" s="17"/>
+    <row r="8" spans="1:53" x14ac:dyDescent="0.35">
+      <c r="A8" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>183</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="9" spans="1:53" x14ac:dyDescent="0.35">
+      <c r="A9" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>184</v>
+      </c>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0"/>
@@ -1900,153 +1922,153 @@
       <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="32.21875" customWidth="1"/>
+    <col min="1" max="1" width="32.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A14" s="2" t="s">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A15" s="2" t="s">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A16" s="2" t="s">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A17" s="2" t="s">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A18" s="2" t="s">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A19" s="2" t="s">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A20" s="2" t="s">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A21" s="2" t="s">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A22" s="2" t="s">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A23" s="2" t="s">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A24" s="2" t="s">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A25" s="2" t="s">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A26" s="2" t="s">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A27" s="2" t="s">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A28" s="2" t="s">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A29" s="2" t="s">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
         <v>133</v>
       </c>
     </row>
@@ -2062,169 +2084,164 @@
   </sheetPr>
   <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.77734375" style="3" hidden="1" customWidth="1"/>
-    <col min="2" max="2" width="30.77734375" style="18" customWidth="1"/>
-    <col min="3" max="3" width="19.77734375" style="18" customWidth="1"/>
-    <col min="4" max="5" width="9.21875" style="18"/>
-    <col min="6" max="6" width="53.77734375" style="18" customWidth="1"/>
-    <col min="7" max="16384" width="9.21875" style="18"/>
+    <col min="1" max="1" width="19.81640625" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="30.81640625" style="10" customWidth="1"/>
+    <col min="3" max="3" width="19.81640625" style="10" customWidth="1"/>
+    <col min="4" max="5" width="9.1796875" style="10"/>
+    <col min="6" max="6" width="53.81640625" style="10" customWidth="1"/>
+    <col min="7" max="16384" width="9.1796875" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="31.2" x14ac:dyDescent="0.6">
-      <c r="A1" s="9"/>
-      <c r="B1" s="23" t="s">
+    <row r="1" spans="1:7" ht="31" x14ac:dyDescent="0.7">
+      <c r="B1" s="15" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="58.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="9"/>
-      <c r="B2" s="35" t="s">
+    <row r="2" spans="1:7" ht="58.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="27" t="s">
         <v>175</v>
       </c>
-      <c r="C2" s="35"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="9"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B4" s="3" t="s">
+      <c r="C2" s="27"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B4" t="s">
         <v>170</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
+    <row r="5" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
         <v>136</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="F5" s="34"/>
-      <c r="G5" s="22"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
+      <c r="F5" s="26"/>
+      <c r="G5" s="14"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
         <v>137</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" t="s">
         <v>150</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="F6" s="34"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
+      <c r="F6" s="26"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
         <v>138</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" t="s">
         <v>149</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="F7" s="34"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="3" t="s">
+      <c r="F7" s="26"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
         <v>139</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" t="s">
         <v>23</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="F8" s="34"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="3" t="s">
+      <c r="F8" s="26"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
         <v>140</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="F9" s="34"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="3" t="s">
+      <c r="F9" s="26"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
         <v>141</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" t="s">
         <v>148</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="F10" s="34"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="3" t="s">
+      <c r="F10" s="26"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
         <v>142</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="3" t="s">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
         <v>143</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" t="s">
         <v>144</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="3" t="s">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
         <v>145</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" t="s">
         <v>146</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="3" t="s">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
         <v>147</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B14" t="s">
         <v>26</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="C14" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" s="9" t="s">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
         <v>178</v>
       </c>
-      <c r="B15" s="9" t="s">
+      <c r="B15" t="s">
         <v>179</v>
       </c>
-      <c r="C15" s="4">
+      <c r="C15" s="2">
         <v>10</v>
       </c>
     </row>
@@ -2260,14 +2277,14 @@
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="23.21875" customWidth="1"/>
-    <col min="2" max="2" width="16.5546875" customWidth="1"/>
-    <col min="3" max="3" width="135.77734375" customWidth="1"/>
+    <col min="1" max="1" width="23.1796875" customWidth="1"/>
+    <col min="2" max="2" width="16.54296875" customWidth="1"/>
+    <col min="3" max="3" width="135.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -2293,30 +2310,29 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="25.21875" style="3" customWidth="1"/>
-    <col min="2" max="2" width="20.77734375" style="3" customWidth="1"/>
-    <col min="3" max="3" width="24.21875" style="3" customWidth="1"/>
-    <col min="4" max="4" width="66.77734375" style="3" customWidth="1"/>
-    <col min="5" max="5" width="26.77734375" style="3" customWidth="1"/>
-    <col min="6" max="16384" width="9.21875" style="3"/>
+    <col min="1" max="1" width="25.1796875" customWidth="1"/>
+    <col min="2" max="2" width="20.81640625" customWidth="1"/>
+    <col min="3" max="3" width="24.1796875" customWidth="1"/>
+    <col min="4" max="4" width="66.81640625" customWidth="1"/>
+    <col min="5" max="5" width="26.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" t="s">
         <v>135</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" t="s">
         <v>134</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" t="s">
         <v>49</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" t="s">
         <v>86</v>
       </c>
     </row>
@@ -2335,36 +2351,36 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="24" customWidth="1"/>
-    <col min="2" max="2" width="25.5546875" customWidth="1"/>
-    <col min="3" max="3" width="11.5546875" customWidth="1"/>
-    <col min="4" max="4" width="44.77734375" customWidth="1"/>
-    <col min="5" max="5" width="15.77734375" customWidth="1"/>
-    <col min="6" max="6" width="22.44140625" customWidth="1"/>
-    <col min="7" max="7" width="21.77734375" customWidth="1"/>
-    <col min="8" max="14" width="16.21875" customWidth="1"/>
-    <col min="15" max="15" width="15.21875" customWidth="1"/>
+    <col min="2" max="2" width="25.54296875" customWidth="1"/>
+    <col min="3" max="3" width="11.54296875" customWidth="1"/>
+    <col min="4" max="4" width="44.81640625" customWidth="1"/>
+    <col min="5" max="5" width="15.81640625" customWidth="1"/>
+    <col min="6" max="6" width="22.453125" customWidth="1"/>
+    <col min="7" max="7" width="21.81640625" customWidth="1"/>
+    <col min="8" max="14" width="16.1796875" customWidth="1"/>
+    <col min="15" max="15" width="15.1796875" customWidth="1"/>
     <col min="16" max="16" width="18" customWidth="1"/>
-    <col min="17" max="17" width="9.21875" style="1"/>
-    <col min="18" max="18" width="15.77734375" customWidth="1"/>
-    <col min="19" max="19" width="13.44140625" customWidth="1"/>
+    <col min="17" max="17" width="9.1796875" style="1"/>
+    <col min="18" max="18" width="15.81640625" customWidth="1"/>
+    <col min="19" max="19" width="13.453125" customWidth="1"/>
     <col min="20" max="20" width="12" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="14" customWidth="1"/>
-    <col min="22" max="22" width="13.21875" customWidth="1"/>
-    <col min="23" max="23" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="11.21875" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="14.77734375" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="10.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="11.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="12.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="14.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="11.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="12.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="13.1796875" customWidth="1"/>
+    <col min="23" max="23" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="14.81640625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="10.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="11.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="12.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="14.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="11.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="12.81640625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -2476,19 +2492,19 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="22" customWidth="1"/>
     <col min="2" max="2" width="21" customWidth="1"/>
-    <col min="3" max="3" width="12.21875" customWidth="1"/>
-    <col min="4" max="4" width="17.21875" customWidth="1"/>
-    <col min="5" max="5" width="17.21875" style="1" customWidth="1"/>
-    <col min="6" max="8" width="17.21875" customWidth="1"/>
-    <col min="9" max="10" width="17.21875" style="1" customWidth="1"/>
-    <col min="11" max="11" width="17.21875" customWidth="1"/>
+    <col min="3" max="3" width="12.1796875" customWidth="1"/>
+    <col min="4" max="4" width="17.1796875" customWidth="1"/>
+    <col min="5" max="5" width="17.1796875" style="1" customWidth="1"/>
+    <col min="6" max="8" width="17.1796875" customWidth="1"/>
+    <col min="9" max="10" width="17.1796875" style="1" customWidth="1"/>
+    <col min="11" max="11" width="17.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -2540,48 +2556,47 @@
       <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="25.21875" style="9" customWidth="1"/>
-    <col min="2" max="2" width="20.77734375" style="9" customWidth="1"/>
-    <col min="3" max="3" width="24.21875" style="9" customWidth="1"/>
-    <col min="4" max="4" width="16.77734375" style="9" customWidth="1"/>
-    <col min="5" max="5" width="20" style="9" customWidth="1"/>
-    <col min="6" max="16384" width="9.21875" style="9"/>
+    <col min="1" max="1" width="25.1796875" customWidth="1"/>
+    <col min="2" max="2" width="20.81640625" customWidth="1"/>
+    <col min="3" max="3" width="24.1796875" customWidth="1"/>
+    <col min="4" max="4" width="16.81640625" customWidth="1"/>
+    <col min="5" max="5" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" t="s">
         <v>159</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" t="s">
         <v>160</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" t="s">
         <v>161</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" t="s">
         <v>162</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" t="s">
         <v>163</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="G1" t="s">
         <v>34</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="H1" t="s">
         <v>164</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="I1" t="s">
         <v>165</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="J1" t="s">
         <v>166</v>
       </c>
-      <c r="K1" s="9" t="s">
+      <c r="K1" t="s">
         <v>167</v>
       </c>
     </row>
@@ -2600,20 +2615,20 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="24.21875" customWidth="1"/>
-    <col min="2" max="2" width="20.77734375" customWidth="1"/>
-    <col min="3" max="3" width="24.44140625" customWidth="1"/>
-    <col min="4" max="4" width="17.77734375" customWidth="1"/>
-    <col min="5" max="5" width="18.77734375" customWidth="1"/>
+    <col min="1" max="1" width="24.1796875" customWidth="1"/>
+    <col min="2" max="2" width="20.81640625" customWidth="1"/>
+    <col min="3" max="3" width="24.453125" customWidth="1"/>
+    <col min="4" max="4" width="17.81640625" customWidth="1"/>
+    <col min="5" max="5" width="18.81640625" customWidth="1"/>
     <col min="6" max="6" width="17" customWidth="1"/>
-    <col min="7" max="7" width="20.77734375" customWidth="1"/>
-    <col min="8" max="8" width="138.5546875" customWidth="1"/>
-    <col min="9" max="9" width="100.44140625" customWidth="1"/>
+    <col min="7" max="7" width="20.81640625" customWidth="1"/>
+    <col min="8" max="8" width="138.54296875" customWidth="1"/>
+    <col min="9" max="9" width="100.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -2657,18 +2672,18 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20.77734375" customWidth="1"/>
+    <col min="1" max="1" width="20.81640625" customWidth="1"/>
     <col min="2" max="2" width="25" customWidth="1"/>
-    <col min="3" max="3" width="16.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.21875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="29.77734375" customWidth="1"/>
+    <col min="3" max="3" width="16.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="29.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -2706,14 +2721,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="26" customWidth="1"/>
-    <col min="2" max="2" width="25.21875" customWidth="1"/>
-    <col min="5" max="5" width="27.77734375" customWidth="1"/>
+    <col min="2" max="2" width="25.1796875" customWidth="1"/>
+    <col min="5" max="5" width="27.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -2747,49 +2762,47 @@
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="24.21875" style="7" customWidth="1"/>
-    <col min="2" max="2" width="24.21875" style="8" customWidth="1"/>
-    <col min="3" max="3" width="20.77734375" style="7" customWidth="1"/>
-    <col min="4" max="4" width="46.77734375" style="7" customWidth="1"/>
-    <col min="5" max="5" width="17.77734375" style="7" customWidth="1"/>
-    <col min="6" max="6" width="30.5546875" style="8" customWidth="1"/>
-    <col min="7" max="7" width="17" style="7" customWidth="1"/>
-    <col min="8" max="8" width="138.5546875" style="7" customWidth="1"/>
-    <col min="9" max="9" width="19" style="7" customWidth="1"/>
-    <col min="10" max="16384" width="9.21875" style="7"/>
+    <col min="1" max="2" width="24.1796875" customWidth="1"/>
+    <col min="3" max="3" width="20.81640625" customWidth="1"/>
+    <col min="4" max="4" width="46.81640625" customWidth="1"/>
+    <col min="5" max="5" width="17.81640625" customWidth="1"/>
+    <col min="6" max="6" width="30.54296875" customWidth="1"/>
+    <col min="7" max="7" width="17" customWidth="1"/>
+    <col min="8" max="8" width="138.54296875" customWidth="1"/>
+    <col min="9" max="9" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" t="s">
         <v>153</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" t="s">
         <v>38</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" t="s">
         <v>39</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" t="s">
         <v>40</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" t="s">
         <v>154</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" t="s">
         <v>42</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="H1" t="s">
         <v>41</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="I1" t="s">
         <v>104</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="J1" t="s">
         <v>155</v>
       </c>
     </row>
@@ -2797,4 +2810,10 @@
   <autoFilter ref="A1:H1" xr:uid="{B7EB6E73-7A47-4B22-A88C-5BA601D79630}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
+<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
+  <clbl:label id="{f956267e-7d50-46d0-9b27-8f911a5b38ff}" enabled="1" method="Standard" siteId="{6c637512-c417-4e78-9d62-b61258e4b619}" contentBits="0" removed="0"/>
+</clbl:labelList>
 </file>
</xml_diff>